<commit_message>
Aggregate to monthly working
</commit_message>
<xml_diff>
--- a/AutoReadUSBRData/USBRWebPortalMetaData.xlsx
+++ b/AutoReadUSBRData/USBRWebPortalMetaData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\AutoReadUSBRData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996F7E78-B98F-4F83-8A62-E4D050F32CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAD6256-C826-40E6-9AFE-7C51020B1CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reservoirs" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>FieldID</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Storage</t>
   </si>
   <si>
-    <t>Acre-feet</t>
-  </si>
-  <si>
     <t>Evaporation</t>
   </si>
   <si>
@@ -101,6 +98,15 @@
   </si>
   <si>
     <t>Mead</t>
+  </si>
+  <si>
+    <t>AggregateByTimePeriod</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4324F4E-C985-4466-9080-C1EEE611FCDF}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -436,13 +442,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -450,10 +456,10 @@
         <v>919</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -461,10 +467,10 @@
         <v>921</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,7 +492,7 @@
     <col min="3" max="3" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,8 +502,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>17</v>
       </c>
@@ -505,106 +514,136 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>29</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>49</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>89</v>
       </c>
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
+      <c r="D11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>